<commit_message>
Few fixes for new release
</commit_message>
<xml_diff>
--- a/csv/Grand Slams Stack.xlsx
+++ b/csv/Grand Slams Stack.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbenj\OneDrive\Bureau\Essais R Shiny\App5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afka\Desktop\R Tennis App\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808B3A91-633C-4158-A367-29F294112919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2715979E-34FB-4AF9-844D-F64146FA83B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13740" yWindow="3795" windowWidth="13125" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2010" yWindow="645" windowWidth="24330" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roger Federer" sheetId="1" r:id="rId1"/>
@@ -42,13 +42,13 @@
     <t>US Open</t>
   </si>
   <si>
-    <t>Rolland Garros</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>Roland Garros</t>
   </si>
 </sst>
 </file>
@@ -536,48 +536,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -593,7 +593,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -891,11 +891,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
@@ -905,13 +905,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
         <v>2009</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1182,7 +1182,7 @@
         <v>2010</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1229,7 +1229,7 @@
         <v>2011</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1276,7 +1276,7 @@
         <v>2012</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1323,7 +1323,7 @@
         <v>2013</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1370,7 +1370,7 @@
         <v>2014</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1417,7 +1417,7 @@
         <v>2015</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1464,7 +1464,7 @@
         <v>2016</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1511,7 +1511,7 @@
         <v>2017</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -1558,7 +1558,7 @@
         <v>2018</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1605,7 +1605,7 @@
         <v>2019</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1652,7 +1652,7 @@
         <v>2020</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -1699,7 +1699,7 @@
         <v>2021</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -1740,10 +1740,10 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
   </cols>
@@ -1753,13 +1753,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1767,7 +1767,7 @@
         <v>2005</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1781,7 +1781,7 @@
         <v>2006</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1795,7 +1795,7 @@
         <v>2007</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1809,7 +1809,7 @@
         <v>2008</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1845,7 +1845,7 @@
         <v>2009</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -1881,7 +1881,7 @@
         <v>2010</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -1928,7 +1928,7 @@
         <v>2011</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -1975,7 +1975,7 @@
         <v>2012</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C19">
         <v>7</v>
@@ -2022,7 +2022,7 @@
         <v>2013</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C23">
         <v>8</v>
@@ -2069,7 +2069,7 @@
         <v>2014</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C27">
         <v>9</v>
@@ -2116,7 +2116,7 @@
         <v>2015</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C31">
         <v>9</v>
@@ -2163,7 +2163,7 @@
         <v>2016</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C35">
         <v>9</v>
@@ -2210,7 +2210,7 @@
         <v>2017</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C39">
         <v>10</v>
@@ -2257,7 +2257,7 @@
         <v>2018</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C43">
         <v>11</v>
@@ -2304,7 +2304,7 @@
         <v>2019</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C47">
         <v>12</v>
@@ -2351,7 +2351,7 @@
         <v>2020</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C51">
         <v>13</v>
@@ -2398,7 +2398,7 @@
         <v>2021</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C55">
         <v>13</v>
@@ -2438,11 +2438,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88540B1B-242E-4275-8493-3BFBB86F3321}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
   </cols>
@@ -2452,13 +2452,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2702,7 +2702,7 @@
         <v>2016</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2749,7 +2749,7 @@
         <v>2017</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2796,7 +2796,7 @@
         <v>2018</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2843,7 +2843,7 @@
         <v>2019</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2890,7 +2890,7 @@
         <v>2020</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2937,7 +2937,7 @@
         <v>2021</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C41">
         <v>2</v>

</xml_diff>